<commit_message>
atualiza com dados até abr/2020
</commit_message>
<xml_diff>
--- a/base-siafi/dados/tg_ Base Siafi 2019 so RGPS Pgtos Totais Esf-Acao-Mod.xlsx
+++ b/base-siafi/dados/tg_ Base Siafi 2019 so RGPS Pgtos Totais Esf-Acao-Mod.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="83">
   <si>
     <t>Base Siafi 2019 so RGPS Pgtos Totais Esf-Acao-Mod</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Item Informação: 56:PAGAMENTOS TOTAIS (EXERCICIO E RAP)</t>
   </si>
   <si>
-    <t>Métrica: Movimento R$ (Item Informação)</t>
+    <t>Métrica: Movim. Líquido - R$ (Item Informação)</t>
   </si>
   <si>
     <t xml:space="preserve">Esfera Orçamentária Código</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Mês Lançamento Número Mês</t>
   </si>
   <si>
-    <t xml:space="preserve">Movimento R$ (Item Informação)</t>
+    <t xml:space="preserve">Movim. Líquido - R$ (Item Informação)</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
@@ -173,6 +173,54 @@
   </si>
   <si>
     <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUL/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGO/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOV/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEZ/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">013/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">014/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
   </si>
   <si>
     <t xml:space="preserve">0625</t>
@@ -263,7 +311,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:U43"/>
+  <dimension ref="A1:U83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -791,7 +839,7 @@
         <v>53</v>
       </c>
       <c r="U16" s="1">
-        <v>9251715.32999992</v>
+        <v>66711422.7800007</v>
       </c>
     </row>
     <row r="17">
@@ -820,43 +868,43 @@
         <v>34</v>
       </c>
       <c r="I17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" t="s">
+        <v>40</v>
+      </c>
+      <c r="O17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>43</v>
+      </c>
+      <c r="R17" t="s">
         <v>54</v>
       </c>
-      <c r="J17" t="s">
+      <c r="S17" t="s">
+        <v>45</v>
+      </c>
+      <c r="T17" t="s">
         <v>55</v>
       </c>
-      <c r="K17" t="s">
-        <v>37</v>
-      </c>
-      <c r="L17" t="s">
-        <v>38</v>
-      </c>
-      <c r="M17" t="s">
-        <v>39</v>
-      </c>
-      <c r="N17" t="s">
-        <v>40</v>
-      </c>
-      <c r="O17" t="s">
-        <v>41</v>
-      </c>
-      <c r="P17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>43</v>
-      </c>
-      <c r="R17" t="s">
-        <v>44</v>
-      </c>
-      <c r="S17" t="s">
-        <v>45</v>
-      </c>
-      <c r="T17" t="s">
-        <v>41</v>
-      </c>
       <c r="U17" s="1">
-        <v>709594360.07</v>
+        <v>113859870.199999</v>
       </c>
     </row>
     <row r="18">
@@ -885,10 +933,10 @@
         <v>34</v>
       </c>
       <c r="I18" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="J18" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="K18" t="s">
         <v>37</v>
@@ -912,16 +960,16 @@
         <v>43</v>
       </c>
       <c r="R18" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="S18" t="s">
         <v>45</v>
       </c>
       <c r="T18" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="U18" s="1">
-        <v>572934223.48</v>
+        <v>131990408.990001</v>
       </c>
     </row>
     <row r="19">
@@ -950,10 +998,10 @@
         <v>34</v>
       </c>
       <c r="I19" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="J19" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="K19" t="s">
         <v>37</v>
@@ -977,16 +1025,16 @@
         <v>43</v>
       </c>
       <c r="R19" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="S19" t="s">
         <v>45</v>
       </c>
       <c r="T19" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="U19" s="1">
-        <v>956666330.04</v>
+        <v>159845842.54</v>
       </c>
     </row>
     <row r="20">
@@ -1015,10 +1063,10 @@
         <v>34</v>
       </c>
       <c r="I20" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="J20" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="K20" t="s">
         <v>37</v>
@@ -1042,16 +1090,16 @@
         <v>43</v>
       </c>
       <c r="R20" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="S20" t="s">
         <v>45</v>
       </c>
       <c r="T20" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="U20" s="1">
-        <v>876046353.92</v>
+        <v>96364292.7399998</v>
       </c>
     </row>
     <row r="21">
@@ -1080,10 +1128,10 @@
         <v>34</v>
       </c>
       <c r="I21" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="J21" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="K21" t="s">
         <v>37</v>
@@ -1107,16 +1155,16 @@
         <v>43</v>
       </c>
       <c r="R21" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="S21" t="s">
         <v>45</v>
       </c>
       <c r="T21" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="U21" s="1">
-        <v>940334079.67</v>
+        <v>57609709.6599998</v>
       </c>
     </row>
     <row r="22">
@@ -1145,10 +1193,10 @@
         <v>34</v>
       </c>
       <c r="I22" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="J22" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="K22" t="s">
         <v>37</v>
@@ -1172,16 +1220,16 @@
         <v>43</v>
       </c>
       <c r="R22" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="S22" t="s">
         <v>45</v>
       </c>
       <c r="T22" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="U22" s="1">
-        <v>25452262.8099999</v>
+        <v>27691794.21</v>
       </c>
     </row>
     <row r="23">
@@ -1192,28 +1240,28 @@
         <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H23" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I23" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="J23" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="K23" t="s">
         <v>37</v>
@@ -1237,16 +1285,16 @@
         <v>43</v>
       </c>
       <c r="R23" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="S23" t="s">
         <v>45</v>
       </c>
       <c r="T23" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="U23" s="1">
-        <v>380741010.29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1257,28 +1305,28 @@
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H24" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I24" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="J24" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="K24" t="s">
         <v>37</v>
@@ -1302,13 +1350,13 @@
         <v>43</v>
       </c>
       <c r="R24" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="S24" t="s">
         <v>45</v>
       </c>
       <c r="T24" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="U24" s="1">
         <v>0</v>
@@ -1322,28 +1370,28 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G25" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H25" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I25" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J25" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="K25" t="s">
         <v>37</v>
@@ -1367,16 +1415,16 @@
         <v>43</v>
       </c>
       <c r="R25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="S25" t="s">
         <v>45</v>
       </c>
       <c r="T25" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="U25" s="1">
-        <v>483053256.24</v>
+        <v>709594360.07</v>
       </c>
     </row>
     <row r="26">
@@ -1387,28 +1435,28 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G26" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H26" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I26" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J26" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="K26" t="s">
         <v>37</v>
@@ -1432,16 +1480,16 @@
         <v>43</v>
       </c>
       <c r="R26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S26" t="s">
         <v>45</v>
       </c>
       <c r="T26" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="U26" s="1">
-        <v>255969667.98</v>
+        <v>572934223.48</v>
       </c>
     </row>
     <row r="27">
@@ -1452,28 +1500,28 @@
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H27" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I27" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J27" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="K27" t="s">
         <v>37</v>
@@ -1497,16 +1545,16 @@
         <v>43</v>
       </c>
       <c r="R27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="S27" t="s">
         <v>45</v>
       </c>
       <c r="T27" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="U27" s="1">
-        <v>242092703.06</v>
+        <v>956666330.04</v>
       </c>
     </row>
     <row r="28">
@@ -1517,28 +1565,28 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G28" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H28" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I28" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J28" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="K28" t="s">
         <v>37</v>
@@ -1562,16 +1610,16 @@
         <v>43</v>
       </c>
       <c r="R28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="S28" t="s">
         <v>45</v>
       </c>
       <c r="T28" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="U28" s="1">
-        <v>283156554.82</v>
+        <v>876046353.92</v>
       </c>
     </row>
     <row r="29">
@@ -1582,28 +1630,28 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E29" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G29" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H29" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I29" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="J29" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K29" t="s">
         <v>37</v>
@@ -1627,16 +1675,16 @@
         <v>43</v>
       </c>
       <c r="R29" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="S29" t="s">
         <v>45</v>
       </c>
       <c r="T29" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="U29" s="1">
-        <v>35532932453.48</v>
+        <v>940334079.67</v>
       </c>
     </row>
     <row r="30">
@@ -1647,28 +1695,28 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G30" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H30" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I30" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="J30" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K30" t="s">
         <v>37</v>
@@ -1692,16 +1740,16 @@
         <v>43</v>
       </c>
       <c r="R30" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="S30" t="s">
         <v>45</v>
       </c>
       <c r="T30" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="U30" s="1">
-        <v>45604902847.01</v>
+        <v>1040578097.16</v>
       </c>
     </row>
     <row r="31">
@@ -1712,28 +1760,28 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G31" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H31" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I31" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="J31" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K31" t="s">
         <v>37</v>
@@ -1757,16 +1805,16 @@
         <v>43</v>
       </c>
       <c r="R31" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="S31" t="s">
         <v>45</v>
       </c>
       <c r="T31" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="U31" s="1">
-        <v>27345470660.24</v>
+        <v>1112253681.75</v>
       </c>
     </row>
     <row r="32">
@@ -1777,61 +1825,61 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" t="s">
+        <v>70</v>
+      </c>
+      <c r="J32" t="s">
+        <v>71</v>
+      </c>
+      <c r="K32" t="s">
+        <v>37</v>
+      </c>
+      <c r="L32" t="s">
+        <v>38</v>
+      </c>
+      <c r="M32" t="s">
+        <v>39</v>
+      </c>
+      <c r="N32" t="s">
+        <v>40</v>
+      </c>
+      <c r="O32" t="s">
+        <v>41</v>
+      </c>
+      <c r="P32" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>43</v>
+      </c>
+      <c r="R32" t="s">
         <v>56</v>
       </c>
-      <c r="D32" t="s">
+      <c r="S32" t="s">
+        <v>45</v>
+      </c>
+      <c r="T32" t="s">
         <v>57</v>
       </c>
-      <c r="E32" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" t="s">
-        <v>59</v>
-      </c>
-      <c r="G32" t="s">
-        <v>60</v>
-      </c>
-      <c r="H32" t="s">
-        <v>57</v>
-      </c>
-      <c r="I32" t="s">
-        <v>63</v>
-      </c>
-      <c r="J32" t="s">
-        <v>64</v>
-      </c>
-      <c r="K32" t="s">
-        <v>37</v>
-      </c>
-      <c r="L32" t="s">
-        <v>38</v>
-      </c>
-      <c r="M32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N32" t="s">
-        <v>40</v>
-      </c>
-      <c r="O32" t="s">
-        <v>41</v>
-      </c>
-      <c r="P32" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>43</v>
-      </c>
-      <c r="R32" t="s">
-        <v>48</v>
-      </c>
-      <c r="S32" t="s">
-        <v>45</v>
-      </c>
-      <c r="T32" t="s">
-        <v>49</v>
-      </c>
       <c r="U32" s="1">
-        <v>36735225735.85</v>
+        <v>1024179744.02</v>
       </c>
     </row>
     <row r="33">
@@ -1842,61 +1890,61 @@
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" t="s">
+        <v>70</v>
+      </c>
+      <c r="J33" t="s">
+        <v>71</v>
+      </c>
+      <c r="K33" t="s">
+        <v>37</v>
+      </c>
+      <c r="L33" t="s">
+        <v>38</v>
+      </c>
+      <c r="M33" t="s">
+        <v>39</v>
+      </c>
+      <c r="N33" t="s">
+        <v>40</v>
+      </c>
+      <c r="O33" t="s">
+        <v>41</v>
+      </c>
+      <c r="P33" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>43</v>
+      </c>
+      <c r="R33" t="s">
         <v>58</v>
       </c>
-      <c r="F33" t="s">
+      <c r="S33" t="s">
+        <v>45</v>
+      </c>
+      <c r="T33" t="s">
         <v>59</v>
       </c>
-      <c r="G33" t="s">
-        <v>60</v>
-      </c>
-      <c r="H33" t="s">
-        <v>57</v>
-      </c>
-      <c r="I33" t="s">
-        <v>63</v>
-      </c>
-      <c r="J33" t="s">
-        <v>64</v>
-      </c>
-      <c r="K33" t="s">
-        <v>37</v>
-      </c>
-      <c r="L33" t="s">
-        <v>38</v>
-      </c>
-      <c r="M33" t="s">
-        <v>39</v>
-      </c>
-      <c r="N33" t="s">
-        <v>40</v>
-      </c>
-      <c r="O33" t="s">
-        <v>41</v>
-      </c>
-      <c r="P33" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>43</v>
-      </c>
-      <c r="R33" t="s">
-        <v>50</v>
-      </c>
-      <c r="S33" t="s">
-        <v>45</v>
-      </c>
-      <c r="T33" t="s">
-        <v>51</v>
-      </c>
       <c r="U33" s="1">
-        <v>36776283820.94</v>
+        <v>1050492697.38</v>
       </c>
     </row>
     <row r="34">
@@ -1907,61 +1955,61 @@
         <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E34" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F34" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" t="s">
+        <v>34</v>
+      </c>
+      <c r="I34" t="s">
+        <v>70</v>
+      </c>
+      <c r="J34" t="s">
+        <v>71</v>
+      </c>
+      <c r="K34" t="s">
+        <v>37</v>
+      </c>
+      <c r="L34" t="s">
+        <v>38</v>
+      </c>
+      <c r="M34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N34" t="s">
+        <v>40</v>
+      </c>
+      <c r="O34" t="s">
+        <v>41</v>
+      </c>
+      <c r="P34" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>43</v>
+      </c>
+      <c r="R34" t="s">
         <v>60</v>
       </c>
-      <c r="H34" t="s">
-        <v>57</v>
-      </c>
-      <c r="I34" t="s">
-        <v>63</v>
-      </c>
-      <c r="J34" t="s">
-        <v>64</v>
-      </c>
-      <c r="K34" t="s">
-        <v>37</v>
-      </c>
-      <c r="L34" t="s">
-        <v>38</v>
-      </c>
-      <c r="M34" t="s">
-        <v>39</v>
-      </c>
-      <c r="N34" t="s">
-        <v>40</v>
-      </c>
-      <c r="O34" t="s">
-        <v>41</v>
-      </c>
-      <c r="P34" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>43</v>
-      </c>
-      <c r="R34" t="s">
-        <v>52</v>
-      </c>
       <c r="S34" t="s">
         <v>45</v>
       </c>
       <c r="T34" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="U34" s="1">
-        <v>31619201138.78</v>
+        <v>1075143852.54</v>
       </c>
     </row>
     <row r="35">
@@ -1972,28 +2020,28 @@
         <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E35" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F35" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G35" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H35" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I35" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J35" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="K35" t="s">
         <v>37</v>
@@ -2017,16 +2065,16 @@
         <v>43</v>
       </c>
       <c r="R35" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="S35" t="s">
         <v>45</v>
       </c>
       <c r="T35" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="U35" s="1">
-        <v>9486339336.77</v>
+        <v>1079045928.42</v>
       </c>
     </row>
     <row r="36">
@@ -2037,61 +2085,61 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F36" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G36" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H36" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I36" t="s">
+        <v>70</v>
+      </c>
+      <c r="J36" t="s">
+        <v>71</v>
+      </c>
+      <c r="K36" t="s">
+        <v>37</v>
+      </c>
+      <c r="L36" t="s">
+        <v>38</v>
+      </c>
+      <c r="M36" t="s">
+        <v>39</v>
+      </c>
+      <c r="N36" t="s">
+        <v>40</v>
+      </c>
+      <c r="O36" t="s">
+        <v>41</v>
+      </c>
+      <c r="P36" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>43</v>
+      </c>
+      <c r="R36" t="s">
+        <v>64</v>
+      </c>
+      <c r="S36" t="s">
+        <v>45</v>
+      </c>
+      <c r="T36" t="s">
         <v>65</v>
       </c>
-      <c r="J36" t="s">
-        <v>66</v>
-      </c>
-      <c r="K36" t="s">
-        <v>37</v>
-      </c>
-      <c r="L36" t="s">
-        <v>38</v>
-      </c>
-      <c r="M36" t="s">
-        <v>39</v>
-      </c>
-      <c r="N36" t="s">
-        <v>40</v>
-      </c>
-      <c r="O36" t="s">
-        <v>41</v>
-      </c>
-      <c r="P36" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>43</v>
-      </c>
-      <c r="R36" t="s">
-        <v>46</v>
-      </c>
-      <c r="S36" t="s">
-        <v>45</v>
-      </c>
-      <c r="T36" t="s">
-        <v>27</v>
-      </c>
       <c r="U36" s="1">
-        <v>567052855.599998</v>
+        <v>883526183.429998</v>
       </c>
     </row>
     <row r="37">
@@ -2102,61 +2150,61 @@
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E37" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F37" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G37" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H37" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I37" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J37" t="s">
+        <v>71</v>
+      </c>
+      <c r="K37" t="s">
+        <v>37</v>
+      </c>
+      <c r="L37" t="s">
+        <v>38</v>
+      </c>
+      <c r="M37" t="s">
+        <v>39</v>
+      </c>
+      <c r="N37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O37" t="s">
+        <v>41</v>
+      </c>
+      <c r="P37" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>43</v>
+      </c>
+      <c r="R37" t="s">
         <v>66</v>
       </c>
-      <c r="K37" t="s">
-        <v>37</v>
-      </c>
-      <c r="L37" t="s">
-        <v>38</v>
-      </c>
-      <c r="M37" t="s">
-        <v>39</v>
-      </c>
-      <c r="N37" t="s">
-        <v>40</v>
-      </c>
-      <c r="O37" t="s">
-        <v>41</v>
-      </c>
-      <c r="P37" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>43</v>
-      </c>
-      <c r="R37" t="s">
-        <v>47</v>
-      </c>
       <c r="S37" t="s">
         <v>45</v>
       </c>
       <c r="T37" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="U37" s="1">
-        <v>18841702314.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -2167,28 +2215,28 @@
         <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="E38" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F38" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G38" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H38" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="I38" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J38" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="K38" t="s">
         <v>37</v>
@@ -2212,16 +2260,16 @@
         <v>43</v>
       </c>
       <c r="R38" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="S38" t="s">
         <v>45</v>
       </c>
       <c r="T38" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="U38" s="1">
-        <v>9735751180.34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -2232,28 +2280,28 @@
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="E39" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F39" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="G39" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="H39" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="I39" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="J39" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="K39" t="s">
         <v>37</v>
@@ -2277,16 +2325,16 @@
         <v>43</v>
       </c>
       <c r="R39" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="S39" t="s">
         <v>45</v>
       </c>
       <c r="T39" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="U39" s="1">
-        <v>9587040690.81</v>
+        <v>380741010.29</v>
       </c>
     </row>
     <row r="40">
@@ -2297,61 +2345,2661 @@
         <v>28</v>
       </c>
       <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" t="s">
+        <v>75</v>
+      </c>
+      <c r="G40" t="s">
+        <v>76</v>
+      </c>
+      <c r="H40" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" t="s">
+        <v>77</v>
+      </c>
+      <c r="J40" t="s">
+        <v>78</v>
+      </c>
+      <c r="K40" t="s">
+        <v>37</v>
+      </c>
+      <c r="L40" t="s">
+        <v>38</v>
+      </c>
+      <c r="M40" t="s">
+        <v>39</v>
+      </c>
+      <c r="N40" t="s">
+        <v>40</v>
+      </c>
+      <c r="O40" t="s">
+        <v>41</v>
+      </c>
+      <c r="P40" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>43</v>
+      </c>
+      <c r="R40" t="s">
+        <v>46</v>
+      </c>
+      <c r="S40" t="s">
+        <v>45</v>
+      </c>
+      <c r="T40" t="s">
+        <v>27</v>
+      </c>
+      <c r="U40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" t="s">
+        <v>74</v>
+      </c>
+      <c r="F41" t="s">
+        <v>75</v>
+      </c>
+      <c r="G41" t="s">
+        <v>76</v>
+      </c>
+      <c r="H41" t="s">
+        <v>73</v>
+      </c>
+      <c r="I41" t="s">
+        <v>77</v>
+      </c>
+      <c r="J41" t="s">
+        <v>78</v>
+      </c>
+      <c r="K41" t="s">
+        <v>37</v>
+      </c>
+      <c r="L41" t="s">
+        <v>38</v>
+      </c>
+      <c r="M41" t="s">
+        <v>39</v>
+      </c>
+      <c r="N41" t="s">
+        <v>40</v>
+      </c>
+      <c r="O41" t="s">
+        <v>41</v>
+      </c>
+      <c r="P41" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>43</v>
+      </c>
+      <c r="R41" t="s">
+        <v>47</v>
+      </c>
+      <c r="S41" t="s">
+        <v>45</v>
+      </c>
+      <c r="T41" t="s">
+        <v>37</v>
+      </c>
+      <c r="U41" s="1">
+        <v>483053256.24</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" t="s">
+        <v>73</v>
+      </c>
+      <c r="I42" t="s">
+        <v>77</v>
+      </c>
+      <c r="J42" t="s">
+        <v>78</v>
+      </c>
+      <c r="K42" t="s">
+        <v>37</v>
+      </c>
+      <c r="L42" t="s">
+        <v>38</v>
+      </c>
+      <c r="M42" t="s">
+        <v>39</v>
+      </c>
+      <c r="N42" t="s">
+        <v>40</v>
+      </c>
+      <c r="O42" t="s">
+        <v>41</v>
+      </c>
+      <c r="P42" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>43</v>
+      </c>
+      <c r="R42" t="s">
+        <v>48</v>
+      </c>
+      <c r="S42" t="s">
+        <v>45</v>
+      </c>
+      <c r="T42" t="s">
+        <v>49</v>
+      </c>
+      <c r="U42" s="1">
+        <v>255969667.98</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" t="s">
+        <v>76</v>
+      </c>
+      <c r="H43" t="s">
+        <v>73</v>
+      </c>
+      <c r="I43" t="s">
+        <v>77</v>
+      </c>
+      <c r="J43" t="s">
+        <v>78</v>
+      </c>
+      <c r="K43" t="s">
+        <v>37</v>
+      </c>
+      <c r="L43" t="s">
+        <v>38</v>
+      </c>
+      <c r="M43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N43" t="s">
+        <v>40</v>
+      </c>
+      <c r="O43" t="s">
+        <v>41</v>
+      </c>
+      <c r="P43" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>43</v>
+      </c>
+      <c r="R43" t="s">
+        <v>50</v>
+      </c>
+      <c r="S43" t="s">
+        <v>45</v>
+      </c>
+      <c r="T43" t="s">
+        <v>51</v>
+      </c>
+      <c r="U43" s="1">
+        <v>242092703.06</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44" t="s">
+        <v>75</v>
+      </c>
+      <c r="G44" t="s">
+        <v>76</v>
+      </c>
+      <c r="H44" t="s">
+        <v>73</v>
+      </c>
+      <c r="I44" t="s">
+        <v>77</v>
+      </c>
+      <c r="J44" t="s">
+        <v>78</v>
+      </c>
+      <c r="K44" t="s">
+        <v>37</v>
+      </c>
+      <c r="L44" t="s">
+        <v>38</v>
+      </c>
+      <c r="M44" t="s">
+        <v>39</v>
+      </c>
+      <c r="N44" t="s">
+        <v>40</v>
+      </c>
+      <c r="O44" t="s">
+        <v>41</v>
+      </c>
+      <c r="P44" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>43</v>
+      </c>
+      <c r="R44" t="s">
+        <v>52</v>
+      </c>
+      <c r="S44" t="s">
+        <v>45</v>
+      </c>
+      <c r="T44" t="s">
+        <v>53</v>
+      </c>
+      <c r="U44" s="1">
+        <v>283156554.82</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" t="s">
+        <v>74</v>
+      </c>
+      <c r="F45" t="s">
+        <v>75</v>
+      </c>
+      <c r="G45" t="s">
+        <v>76</v>
+      </c>
+      <c r="H45" t="s">
+        <v>73</v>
+      </c>
+      <c r="I45" t="s">
+        <v>77</v>
+      </c>
+      <c r="J45" t="s">
+        <v>78</v>
+      </c>
+      <c r="K45" t="s">
+        <v>37</v>
+      </c>
+      <c r="L45" t="s">
+        <v>38</v>
+      </c>
+      <c r="M45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O45" t="s">
+        <v>41</v>
+      </c>
+      <c r="P45" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>43</v>
+      </c>
+      <c r="R45" t="s">
+        <v>54</v>
+      </c>
+      <c r="S45" t="s">
+        <v>45</v>
+      </c>
+      <c r="T45" t="s">
+        <v>55</v>
+      </c>
+      <c r="U45" s="1">
+        <v>233776262.41</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" t="s">
+        <v>75</v>
+      </c>
+      <c r="G46" t="s">
+        <v>76</v>
+      </c>
+      <c r="H46" t="s">
+        <v>73</v>
+      </c>
+      <c r="I46" t="s">
+        <v>77</v>
+      </c>
+      <c r="J46" t="s">
+        <v>78</v>
+      </c>
+      <c r="K46" t="s">
+        <v>37</v>
+      </c>
+      <c r="L46" t="s">
+        <v>38</v>
+      </c>
+      <c r="M46" t="s">
+        <v>39</v>
+      </c>
+      <c r="N46" t="s">
+        <v>40</v>
+      </c>
+      <c r="O46" t="s">
+        <v>41</v>
+      </c>
+      <c r="P46" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>43</v>
+      </c>
+      <c r="R46" t="s">
         <v>56</v>
       </c>
-      <c r="D40" t="s">
+      <c r="S46" t="s">
+        <v>45</v>
+      </c>
+      <c r="T46" t="s">
         <v>57</v>
       </c>
-      <c r="E40" t="s">
+      <c r="U46" s="1">
+        <v>275471745.86</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47" t="s">
+        <v>76</v>
+      </c>
+      <c r="H47" t="s">
+        <v>73</v>
+      </c>
+      <c r="I47" t="s">
+        <v>77</v>
+      </c>
+      <c r="J47" t="s">
+        <v>78</v>
+      </c>
+      <c r="K47" t="s">
+        <v>37</v>
+      </c>
+      <c r="L47" t="s">
+        <v>38</v>
+      </c>
+      <c r="M47" t="s">
+        <v>39</v>
+      </c>
+      <c r="N47" t="s">
+        <v>40</v>
+      </c>
+      <c r="O47" t="s">
+        <v>41</v>
+      </c>
+      <c r="P47" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>43</v>
+      </c>
+      <c r="R47" t="s">
         <v>58</v>
       </c>
-      <c r="F40" t="s">
+      <c r="S47" t="s">
+        <v>45</v>
+      </c>
+      <c r="T47" t="s">
         <v>59</v>
       </c>
-      <c r="G40" t="s">
+      <c r="U47" s="1">
+        <v>277424508.17</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" t="s">
+        <v>74</v>
+      </c>
+      <c r="F48" t="s">
+        <v>75</v>
+      </c>
+      <c r="G48" t="s">
+        <v>76</v>
+      </c>
+      <c r="H48" t="s">
+        <v>73</v>
+      </c>
+      <c r="I48" t="s">
+        <v>77</v>
+      </c>
+      <c r="J48" t="s">
+        <v>78</v>
+      </c>
+      <c r="K48" t="s">
+        <v>37</v>
+      </c>
+      <c r="L48" t="s">
+        <v>38</v>
+      </c>
+      <c r="M48" t="s">
+        <v>39</v>
+      </c>
+      <c r="N48" t="s">
+        <v>40</v>
+      </c>
+      <c r="O48" t="s">
+        <v>41</v>
+      </c>
+      <c r="P48" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>43</v>
+      </c>
+      <c r="R48" t="s">
         <v>60</v>
       </c>
-      <c r="H40" t="s">
+      <c r="S48" t="s">
+        <v>45</v>
+      </c>
+      <c r="T48" t="s">
+        <v>61</v>
+      </c>
+      <c r="U48" s="1">
+        <v>231466790.6</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" t="s">
+        <v>74</v>
+      </c>
+      <c r="F49" t="s">
+        <v>75</v>
+      </c>
+      <c r="G49" t="s">
+        <v>76</v>
+      </c>
+      <c r="H49" t="s">
+        <v>73</v>
+      </c>
+      <c r="I49" t="s">
+        <v>77</v>
+      </c>
+      <c r="J49" t="s">
+        <v>78</v>
+      </c>
+      <c r="K49" t="s">
+        <v>37</v>
+      </c>
+      <c r="L49" t="s">
+        <v>38</v>
+      </c>
+      <c r="M49" t="s">
+        <v>39</v>
+      </c>
+      <c r="N49" t="s">
+        <v>40</v>
+      </c>
+      <c r="O49" t="s">
+        <v>41</v>
+      </c>
+      <c r="P49" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>43</v>
+      </c>
+      <c r="R49" t="s">
+        <v>62</v>
+      </c>
+      <c r="S49" t="s">
+        <v>45</v>
+      </c>
+      <c r="T49" t="s">
+        <v>63</v>
+      </c>
+      <c r="U49" s="1">
+        <v>270420238.64</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" t="s">
+        <v>75</v>
+      </c>
+      <c r="G50" t="s">
+        <v>76</v>
+      </c>
+      <c r="H50" t="s">
+        <v>73</v>
+      </c>
+      <c r="I50" t="s">
+        <v>77</v>
+      </c>
+      <c r="J50" t="s">
+        <v>78</v>
+      </c>
+      <c r="K50" t="s">
+        <v>37</v>
+      </c>
+      <c r="L50" t="s">
+        <v>38</v>
+      </c>
+      <c r="M50" t="s">
+        <v>39</v>
+      </c>
+      <c r="N50" t="s">
+        <v>40</v>
+      </c>
+      <c r="O50" t="s">
+        <v>41</v>
+      </c>
+      <c r="P50" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>43</v>
+      </c>
+      <c r="R50" t="s">
+        <v>64</v>
+      </c>
+      <c r="S50" t="s">
+        <v>45</v>
+      </c>
+      <c r="T50" t="s">
+        <v>65</v>
+      </c>
+      <c r="U50" s="1">
+        <v>426291947.94</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" t="s">
+        <v>75</v>
+      </c>
+      <c r="G51" t="s">
+        <v>76</v>
+      </c>
+      <c r="H51" t="s">
+        <v>73</v>
+      </c>
+      <c r="I51" t="s">
+        <v>77</v>
+      </c>
+      <c r="J51" t="s">
+        <v>78</v>
+      </c>
+      <c r="K51" t="s">
+        <v>37</v>
+      </c>
+      <c r="L51" t="s">
+        <v>38</v>
+      </c>
+      <c r="M51" t="s">
+        <v>39</v>
+      </c>
+      <c r="N51" t="s">
+        <v>40</v>
+      </c>
+      <c r="O51" t="s">
+        <v>41</v>
+      </c>
+      <c r="P51" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>43</v>
+      </c>
+      <c r="R51" t="s">
+        <v>66</v>
+      </c>
+      <c r="S51" t="s">
+        <v>45</v>
+      </c>
+      <c r="T51" t="s">
+        <v>67</v>
+      </c>
+      <c r="U51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" t="s">
+        <v>74</v>
+      </c>
+      <c r="F52" t="s">
+        <v>75</v>
+      </c>
+      <c r="G52" t="s">
+        <v>76</v>
+      </c>
+      <c r="H52" t="s">
+        <v>73</v>
+      </c>
+      <c r="I52" t="s">
+        <v>77</v>
+      </c>
+      <c r="J52" t="s">
+        <v>78</v>
+      </c>
+      <c r="K52" t="s">
+        <v>37</v>
+      </c>
+      <c r="L52" t="s">
+        <v>38</v>
+      </c>
+      <c r="M52" t="s">
+        <v>39</v>
+      </c>
+      <c r="N52" t="s">
+        <v>40</v>
+      </c>
+      <c r="O52" t="s">
+        <v>41</v>
+      </c>
+      <c r="P52" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>43</v>
+      </c>
+      <c r="R52" t="s">
+        <v>68</v>
+      </c>
+      <c r="S52" t="s">
+        <v>45</v>
+      </c>
+      <c r="T52" t="s">
+        <v>69</v>
+      </c>
+      <c r="U52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" t="s">
+        <v>75</v>
+      </c>
+      <c r="G53" t="s">
+        <v>76</v>
+      </c>
+      <c r="H53" t="s">
+        <v>73</v>
+      </c>
+      <c r="I53" t="s">
+        <v>79</v>
+      </c>
+      <c r="J53" t="s">
+        <v>80</v>
+      </c>
+      <c r="K53" t="s">
+        <v>37</v>
+      </c>
+      <c r="L53" t="s">
+        <v>38</v>
+      </c>
+      <c r="M53" t="s">
+        <v>39</v>
+      </c>
+      <c r="N53" t="s">
+        <v>40</v>
+      </c>
+      <c r="O53" t="s">
+        <v>41</v>
+      </c>
+      <c r="P53" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>43</v>
+      </c>
+      <c r="R53" t="s">
+        <v>44</v>
+      </c>
+      <c r="S53" t="s">
+        <v>45</v>
+      </c>
+      <c r="T53" t="s">
+        <v>41</v>
+      </c>
+      <c r="U53" s="1">
+        <v>35532932453.48</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" t="s">
+        <v>74</v>
+      </c>
+      <c r="F54" t="s">
+        <v>75</v>
+      </c>
+      <c r="G54" t="s">
+        <v>76</v>
+      </c>
+      <c r="H54" t="s">
+        <v>73</v>
+      </c>
+      <c r="I54" t="s">
+        <v>79</v>
+      </c>
+      <c r="J54" t="s">
+        <v>80</v>
+      </c>
+      <c r="K54" t="s">
+        <v>37</v>
+      </c>
+      <c r="L54" t="s">
+        <v>38</v>
+      </c>
+      <c r="M54" t="s">
+        <v>39</v>
+      </c>
+      <c r="N54" t="s">
+        <v>40</v>
+      </c>
+      <c r="O54" t="s">
+        <v>41</v>
+      </c>
+      <c r="P54" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>43</v>
+      </c>
+      <c r="R54" t="s">
+        <v>46</v>
+      </c>
+      <c r="S54" t="s">
+        <v>45</v>
+      </c>
+      <c r="T54" t="s">
+        <v>27</v>
+      </c>
+      <c r="U54" s="1">
+        <v>45604902847.01</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" t="s">
+        <v>75</v>
+      </c>
+      <c r="G55" t="s">
+        <v>76</v>
+      </c>
+      <c r="H55" t="s">
+        <v>73</v>
+      </c>
+      <c r="I55" t="s">
+        <v>79</v>
+      </c>
+      <c r="J55" t="s">
+        <v>80</v>
+      </c>
+      <c r="K55" t="s">
+        <v>37</v>
+      </c>
+      <c r="L55" t="s">
+        <v>38</v>
+      </c>
+      <c r="M55" t="s">
+        <v>39</v>
+      </c>
+      <c r="N55" t="s">
+        <v>40</v>
+      </c>
+      <c r="O55" t="s">
+        <v>41</v>
+      </c>
+      <c r="P55" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>43</v>
+      </c>
+      <c r="R55" t="s">
+        <v>47</v>
+      </c>
+      <c r="S55" t="s">
+        <v>45</v>
+      </c>
+      <c r="T55" t="s">
+        <v>37</v>
+      </c>
+      <c r="U55" s="1">
+        <v>27345470660.24</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" t="s">
+        <v>73</v>
+      </c>
+      <c r="E56" t="s">
+        <v>74</v>
+      </c>
+      <c r="F56" t="s">
+        <v>75</v>
+      </c>
+      <c r="G56" t="s">
+        <v>76</v>
+      </c>
+      <c r="H56" t="s">
+        <v>73</v>
+      </c>
+      <c r="I56" t="s">
+        <v>79</v>
+      </c>
+      <c r="J56" t="s">
+        <v>80</v>
+      </c>
+      <c r="K56" t="s">
+        <v>37</v>
+      </c>
+      <c r="L56" t="s">
+        <v>38</v>
+      </c>
+      <c r="M56" t="s">
+        <v>39</v>
+      </c>
+      <c r="N56" t="s">
+        <v>40</v>
+      </c>
+      <c r="O56" t="s">
+        <v>41</v>
+      </c>
+      <c r="P56" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>43</v>
+      </c>
+      <c r="R56" t="s">
+        <v>48</v>
+      </c>
+      <c r="S56" t="s">
+        <v>45</v>
+      </c>
+      <c r="T56" t="s">
+        <v>49</v>
+      </c>
+      <c r="U56" s="1">
+        <v>36735225735.85</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" t="s">
+        <v>74</v>
+      </c>
+      <c r="F57" t="s">
+        <v>75</v>
+      </c>
+      <c r="G57" t="s">
+        <v>76</v>
+      </c>
+      <c r="H57" t="s">
+        <v>73</v>
+      </c>
+      <c r="I57" t="s">
+        <v>79</v>
+      </c>
+      <c r="J57" t="s">
+        <v>80</v>
+      </c>
+      <c r="K57" t="s">
+        <v>37</v>
+      </c>
+      <c r="L57" t="s">
+        <v>38</v>
+      </c>
+      <c r="M57" t="s">
+        <v>39</v>
+      </c>
+      <c r="N57" t="s">
+        <v>40</v>
+      </c>
+      <c r="O57" t="s">
+        <v>41</v>
+      </c>
+      <c r="P57" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>43</v>
+      </c>
+      <c r="R57" t="s">
+        <v>50</v>
+      </c>
+      <c r="S57" t="s">
+        <v>45</v>
+      </c>
+      <c r="T57" t="s">
+        <v>51</v>
+      </c>
+      <c r="U57" s="1">
+        <v>36776283820.94</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" t="s">
+        <v>75</v>
+      </c>
+      <c r="G58" t="s">
+        <v>76</v>
+      </c>
+      <c r="H58" t="s">
+        <v>73</v>
+      </c>
+      <c r="I58" t="s">
+        <v>79</v>
+      </c>
+      <c r="J58" t="s">
+        <v>80</v>
+      </c>
+      <c r="K58" t="s">
+        <v>37</v>
+      </c>
+      <c r="L58" t="s">
+        <v>38</v>
+      </c>
+      <c r="M58" t="s">
+        <v>39</v>
+      </c>
+      <c r="N58" t="s">
+        <v>40</v>
+      </c>
+      <c r="O58" t="s">
+        <v>41</v>
+      </c>
+      <c r="P58" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>43</v>
+      </c>
+      <c r="R58" t="s">
+        <v>52</v>
+      </c>
+      <c r="S58" t="s">
+        <v>45</v>
+      </c>
+      <c r="T58" t="s">
+        <v>53</v>
+      </c>
+      <c r="U58" s="1">
+        <v>36577735574.47</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" t="s">
+        <v>74</v>
+      </c>
+      <c r="F59" t="s">
+        <v>75</v>
+      </c>
+      <c r="G59" t="s">
+        <v>76</v>
+      </c>
+      <c r="H59" t="s">
+        <v>73</v>
+      </c>
+      <c r="I59" t="s">
+        <v>79</v>
+      </c>
+      <c r="J59" t="s">
+        <v>80</v>
+      </c>
+      <c r="K59" t="s">
+        <v>37</v>
+      </c>
+      <c r="L59" t="s">
+        <v>38</v>
+      </c>
+      <c r="M59" t="s">
+        <v>39</v>
+      </c>
+      <c r="N59" t="s">
+        <v>40</v>
+      </c>
+      <c r="O59" t="s">
+        <v>41</v>
+      </c>
+      <c r="P59" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>43</v>
+      </c>
+      <c r="R59" t="s">
+        <v>54</v>
+      </c>
+      <c r="S59" t="s">
+        <v>45</v>
+      </c>
+      <c r="T59" t="s">
+        <v>55</v>
+      </c>
+      <c r="U59" s="1">
+        <v>37080892013.12</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" t="s">
+        <v>72</v>
+      </c>
+      <c r="D60" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" t="s">
+        <v>74</v>
+      </c>
+      <c r="F60" t="s">
+        <v>75</v>
+      </c>
+      <c r="G60" t="s">
+        <v>76</v>
+      </c>
+      <c r="H60" t="s">
+        <v>73</v>
+      </c>
+      <c r="I60" t="s">
+        <v>79</v>
+      </c>
+      <c r="J60" t="s">
+        <v>80</v>
+      </c>
+      <c r="K60" t="s">
+        <v>37</v>
+      </c>
+      <c r="L60" t="s">
+        <v>38</v>
+      </c>
+      <c r="M60" t="s">
+        <v>39</v>
+      </c>
+      <c r="N60" t="s">
+        <v>40</v>
+      </c>
+      <c r="O60" t="s">
+        <v>41</v>
+      </c>
+      <c r="P60" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>43</v>
+      </c>
+      <c r="R60" t="s">
+        <v>56</v>
+      </c>
+      <c r="S60" t="s">
+        <v>45</v>
+      </c>
+      <c r="T60" t="s">
         <v>57</v>
       </c>
-      <c r="I40" t="s">
+      <c r="U60" s="1">
+        <v>39789523090.16</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61" t="s">
+        <v>72</v>
+      </c>
+      <c r="D61" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" t="s">
+        <v>75</v>
+      </c>
+      <c r="G61" t="s">
+        <v>76</v>
+      </c>
+      <c r="H61" t="s">
+        <v>73</v>
+      </c>
+      <c r="I61" t="s">
+        <v>79</v>
+      </c>
+      <c r="J61" t="s">
+        <v>80</v>
+      </c>
+      <c r="K61" t="s">
+        <v>37</v>
+      </c>
+      <c r="L61" t="s">
+        <v>38</v>
+      </c>
+      <c r="M61" t="s">
+        <v>39</v>
+      </c>
+      <c r="N61" t="s">
+        <v>40</v>
+      </c>
+      <c r="O61" t="s">
+        <v>41</v>
+      </c>
+      <c r="P61" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>43</v>
+      </c>
+      <c r="R61" t="s">
+        <v>58</v>
+      </c>
+      <c r="S61" t="s">
+        <v>45</v>
+      </c>
+      <c r="T61" t="s">
+        <v>59</v>
+      </c>
+      <c r="U61" s="1">
+        <v>52655279774.68</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" t="s">
+        <v>73</v>
+      </c>
+      <c r="E62" t="s">
+        <v>74</v>
+      </c>
+      <c r="F62" t="s">
+        <v>75</v>
+      </c>
+      <c r="G62" t="s">
+        <v>76</v>
+      </c>
+      <c r="H62" t="s">
+        <v>73</v>
+      </c>
+      <c r="I62" t="s">
+        <v>79</v>
+      </c>
+      <c r="J62" t="s">
+        <v>80</v>
+      </c>
+      <c r="K62" t="s">
+        <v>37</v>
+      </c>
+      <c r="L62" t="s">
+        <v>38</v>
+      </c>
+      <c r="M62" t="s">
+        <v>39</v>
+      </c>
+      <c r="N62" t="s">
+        <v>40</v>
+      </c>
+      <c r="O62" t="s">
+        <v>41</v>
+      </c>
+      <c r="P62" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>43</v>
+      </c>
+      <c r="R62" t="s">
+        <v>60</v>
+      </c>
+      <c r="S62" t="s">
+        <v>45</v>
+      </c>
+      <c r="T62" t="s">
+        <v>61</v>
+      </c>
+      <c r="U62" s="1">
+        <v>37338486165.64</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63" t="s">
+        <v>72</v>
+      </c>
+      <c r="D63" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" t="s">
+        <v>75</v>
+      </c>
+      <c r="G63" t="s">
+        <v>76</v>
+      </c>
+      <c r="H63" t="s">
+        <v>73</v>
+      </c>
+      <c r="I63" t="s">
+        <v>79</v>
+      </c>
+      <c r="J63" t="s">
+        <v>80</v>
+      </c>
+      <c r="K63" t="s">
+        <v>37</v>
+      </c>
+      <c r="L63" t="s">
+        <v>38</v>
+      </c>
+      <c r="M63" t="s">
+        <v>39</v>
+      </c>
+      <c r="N63" t="s">
+        <v>40</v>
+      </c>
+      <c r="O63" t="s">
+        <v>41</v>
+      </c>
+      <c r="P63" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>43</v>
+      </c>
+      <c r="R63" t="s">
+        <v>62</v>
+      </c>
+      <c r="S63" t="s">
+        <v>45</v>
+      </c>
+      <c r="T63" t="s">
+        <v>63</v>
+      </c>
+      <c r="U63" s="1">
+        <v>39885376839.12</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" t="s">
+        <v>72</v>
+      </c>
+      <c r="D64" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" t="s">
+        <v>75</v>
+      </c>
+      <c r="G64" t="s">
+        <v>76</v>
+      </c>
+      <c r="H64" t="s">
+        <v>73</v>
+      </c>
+      <c r="I64" t="s">
+        <v>79</v>
+      </c>
+      <c r="J64" t="s">
+        <v>80</v>
+      </c>
+      <c r="K64" t="s">
+        <v>37</v>
+      </c>
+      <c r="L64" t="s">
+        <v>38</v>
+      </c>
+      <c r="M64" t="s">
+        <v>39</v>
+      </c>
+      <c r="N64" t="s">
+        <v>40</v>
+      </c>
+      <c r="O64" t="s">
+        <v>41</v>
+      </c>
+      <c r="P64" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>43</v>
+      </c>
+      <c r="R64" t="s">
+        <v>64</v>
+      </c>
+      <c r="S64" t="s">
+        <v>45</v>
+      </c>
+      <c r="T64" t="s">
         <v>65</v>
       </c>
-      <c r="J40" t="s">
+      <c r="U64" s="1">
+        <v>53137925022.5699</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65" t="s">
+        <v>28</v>
+      </c>
+      <c r="C65" t="s">
+        <v>72</v>
+      </c>
+      <c r="D65" t="s">
+        <v>73</v>
+      </c>
+      <c r="E65" t="s">
+        <v>74</v>
+      </c>
+      <c r="F65" t="s">
+        <v>75</v>
+      </c>
+      <c r="G65" t="s">
+        <v>76</v>
+      </c>
+      <c r="H65" t="s">
+        <v>73</v>
+      </c>
+      <c r="I65" t="s">
+        <v>79</v>
+      </c>
+      <c r="J65" t="s">
+        <v>80</v>
+      </c>
+      <c r="K65" t="s">
+        <v>37</v>
+      </c>
+      <c r="L65" t="s">
+        <v>38</v>
+      </c>
+      <c r="M65" t="s">
+        <v>39</v>
+      </c>
+      <c r="N65" t="s">
+        <v>40</v>
+      </c>
+      <c r="O65" t="s">
+        <v>41</v>
+      </c>
+      <c r="P65" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>43</v>
+      </c>
+      <c r="R65" t="s">
         <v>66</v>
       </c>
-      <c r="K40" t="s">
-        <v>37</v>
-      </c>
-      <c r="L40" t="s">
-        <v>38</v>
-      </c>
-      <c r="M40" t="s">
-        <v>39</v>
-      </c>
-      <c r="N40" t="s">
-        <v>40</v>
-      </c>
-      <c r="O40" t="s">
-        <v>41</v>
-      </c>
-      <c r="P40" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>43</v>
-      </c>
-      <c r="R40" t="s">
+      <c r="S65" t="s">
+        <v>45</v>
+      </c>
+      <c r="T65" t="s">
+        <v>67</v>
+      </c>
+      <c r="U65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" t="s">
+        <v>73</v>
+      </c>
+      <c r="E66" t="s">
+        <v>74</v>
+      </c>
+      <c r="F66" t="s">
+        <v>75</v>
+      </c>
+      <c r="G66" t="s">
+        <v>76</v>
+      </c>
+      <c r="H66" t="s">
+        <v>73</v>
+      </c>
+      <c r="I66" t="s">
+        <v>79</v>
+      </c>
+      <c r="J66" t="s">
+        <v>80</v>
+      </c>
+      <c r="K66" t="s">
+        <v>37</v>
+      </c>
+      <c r="L66" t="s">
+        <v>38</v>
+      </c>
+      <c r="M66" t="s">
+        <v>39</v>
+      </c>
+      <c r="N66" t="s">
+        <v>40</v>
+      </c>
+      <c r="O66" t="s">
+        <v>41</v>
+      </c>
+      <c r="P66" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>43</v>
+      </c>
+      <c r="R66" t="s">
+        <v>68</v>
+      </c>
+      <c r="S66" t="s">
+        <v>45</v>
+      </c>
+      <c r="T66" t="s">
+        <v>69</v>
+      </c>
+      <c r="U66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" t="s">
+        <v>73</v>
+      </c>
+      <c r="E67" t="s">
+        <v>74</v>
+      </c>
+      <c r="F67" t="s">
+        <v>75</v>
+      </c>
+      <c r="G67" t="s">
+        <v>76</v>
+      </c>
+      <c r="H67" t="s">
+        <v>73</v>
+      </c>
+      <c r="I67" t="s">
+        <v>81</v>
+      </c>
+      <c r="J67" t="s">
+        <v>82</v>
+      </c>
+      <c r="K67" t="s">
+        <v>37</v>
+      </c>
+      <c r="L67" t="s">
+        <v>38</v>
+      </c>
+      <c r="M67" t="s">
+        <v>39</v>
+      </c>
+      <c r="N67" t="s">
+        <v>40</v>
+      </c>
+      <c r="O67" t="s">
+        <v>41</v>
+      </c>
+      <c r="P67" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>43</v>
+      </c>
+      <c r="R67" t="s">
+        <v>44</v>
+      </c>
+      <c r="S67" t="s">
+        <v>45</v>
+      </c>
+      <c r="T67" t="s">
+        <v>41</v>
+      </c>
+      <c r="U67" s="1">
+        <v>9486339336.77</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68" t="s">
+        <v>28</v>
+      </c>
+      <c r="C68" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68" t="s">
+        <v>73</v>
+      </c>
+      <c r="E68" t="s">
+        <v>74</v>
+      </c>
+      <c r="F68" t="s">
+        <v>75</v>
+      </c>
+      <c r="G68" t="s">
+        <v>76</v>
+      </c>
+      <c r="H68" t="s">
+        <v>73</v>
+      </c>
+      <c r="I68" t="s">
+        <v>81</v>
+      </c>
+      <c r="J68" t="s">
+        <v>82</v>
+      </c>
+      <c r="K68" t="s">
+        <v>37</v>
+      </c>
+      <c r="L68" t="s">
+        <v>38</v>
+      </c>
+      <c r="M68" t="s">
+        <v>39</v>
+      </c>
+      <c r="N68" t="s">
+        <v>40</v>
+      </c>
+      <c r="O68" t="s">
+        <v>41</v>
+      </c>
+      <c r="P68" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>43</v>
+      </c>
+      <c r="R68" t="s">
+        <v>46</v>
+      </c>
+      <c r="S68" t="s">
+        <v>45</v>
+      </c>
+      <c r="T68" t="s">
+        <v>27</v>
+      </c>
+      <c r="U68" s="1">
+        <v>567052855.599998</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>27</v>
+      </c>
+      <c r="B69" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69" t="s">
+        <v>72</v>
+      </c>
+      <c r="D69" t="s">
+        <v>73</v>
+      </c>
+      <c r="E69" t="s">
+        <v>74</v>
+      </c>
+      <c r="F69" t="s">
+        <v>75</v>
+      </c>
+      <c r="G69" t="s">
+        <v>76</v>
+      </c>
+      <c r="H69" t="s">
+        <v>73</v>
+      </c>
+      <c r="I69" t="s">
+        <v>81</v>
+      </c>
+      <c r="J69" t="s">
+        <v>82</v>
+      </c>
+      <c r="K69" t="s">
+        <v>37</v>
+      </c>
+      <c r="L69" t="s">
+        <v>38</v>
+      </c>
+      <c r="M69" t="s">
+        <v>39</v>
+      </c>
+      <c r="N69" t="s">
+        <v>40</v>
+      </c>
+      <c r="O69" t="s">
+        <v>41</v>
+      </c>
+      <c r="P69" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>43</v>
+      </c>
+      <c r="R69" t="s">
+        <v>47</v>
+      </c>
+      <c r="S69" t="s">
+        <v>45</v>
+      </c>
+      <c r="T69" t="s">
+        <v>37</v>
+      </c>
+      <c r="U69" s="1">
+        <v>18841702314.3</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" t="s">
+        <v>74</v>
+      </c>
+      <c r="F70" t="s">
+        <v>75</v>
+      </c>
+      <c r="G70" t="s">
+        <v>76</v>
+      </c>
+      <c r="H70" t="s">
+        <v>73</v>
+      </c>
+      <c r="I70" t="s">
+        <v>81</v>
+      </c>
+      <c r="J70" t="s">
+        <v>82</v>
+      </c>
+      <c r="K70" t="s">
+        <v>37</v>
+      </c>
+      <c r="L70" t="s">
+        <v>38</v>
+      </c>
+      <c r="M70" t="s">
+        <v>39</v>
+      </c>
+      <c r="N70" t="s">
+        <v>40</v>
+      </c>
+      <c r="O70" t="s">
+        <v>41</v>
+      </c>
+      <c r="P70" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>43</v>
+      </c>
+      <c r="R70" t="s">
+        <v>48</v>
+      </c>
+      <c r="S70" t="s">
+        <v>45</v>
+      </c>
+      <c r="T70" t="s">
+        <v>49</v>
+      </c>
+      <c r="U70" s="1">
+        <v>9735751180.34</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" t="s">
+        <v>28</v>
+      </c>
+      <c r="C71" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" t="s">
+        <v>73</v>
+      </c>
+      <c r="E71" t="s">
+        <v>74</v>
+      </c>
+      <c r="F71" t="s">
+        <v>75</v>
+      </c>
+      <c r="G71" t="s">
+        <v>76</v>
+      </c>
+      <c r="H71" t="s">
+        <v>73</v>
+      </c>
+      <c r="I71" t="s">
+        <v>81</v>
+      </c>
+      <c r="J71" t="s">
+        <v>82</v>
+      </c>
+      <c r="K71" t="s">
+        <v>37</v>
+      </c>
+      <c r="L71" t="s">
+        <v>38</v>
+      </c>
+      <c r="M71" t="s">
+        <v>39</v>
+      </c>
+      <c r="N71" t="s">
+        <v>40</v>
+      </c>
+      <c r="O71" t="s">
+        <v>41</v>
+      </c>
+      <c r="P71" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>43</v>
+      </c>
+      <c r="R71" t="s">
+        <v>50</v>
+      </c>
+      <c r="S71" t="s">
+        <v>45</v>
+      </c>
+      <c r="T71" t="s">
+        <v>51</v>
+      </c>
+      <c r="U71" s="1">
+        <v>9587040690.81</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>27</v>
+      </c>
+      <c r="B72" t="s">
+        <v>28</v>
+      </c>
+      <c r="C72" t="s">
+        <v>72</v>
+      </c>
+      <c r="D72" t="s">
+        <v>73</v>
+      </c>
+      <c r="E72" t="s">
+        <v>74</v>
+      </c>
+      <c r="F72" t="s">
+        <v>75</v>
+      </c>
+      <c r="G72" t="s">
+        <v>76</v>
+      </c>
+      <c r="H72" t="s">
+        <v>73</v>
+      </c>
+      <c r="I72" t="s">
+        <v>81</v>
+      </c>
+      <c r="J72" t="s">
+        <v>82</v>
+      </c>
+      <c r="K72" t="s">
+        <v>37</v>
+      </c>
+      <c r="L72" t="s">
+        <v>38</v>
+      </c>
+      <c r="M72" t="s">
+        <v>39</v>
+      </c>
+      <c r="N72" t="s">
+        <v>40</v>
+      </c>
+      <c r="O72" t="s">
+        <v>41</v>
+      </c>
+      <c r="P72" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>43</v>
+      </c>
+      <c r="R72" t="s">
         <v>52</v>
       </c>
-      <c r="S40" t="s">
-        <v>45</v>
-      </c>
-      <c r="T40" t="s">
+      <c r="S72" t="s">
+        <v>45</v>
+      </c>
+      <c r="T72" t="s">
         <v>53</v>
       </c>
-      <c r="U40" s="1">
-        <v>5008188970.76</v>
+      <c r="U72" s="1">
+        <v>9762880062.46</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>27</v>
+      </c>
+      <c r="B73" t="s">
+        <v>28</v>
+      </c>
+      <c r="C73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D73" t="s">
+        <v>73</v>
+      </c>
+      <c r="E73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F73" t="s">
+        <v>75</v>
+      </c>
+      <c r="G73" t="s">
+        <v>76</v>
+      </c>
+      <c r="H73" t="s">
+        <v>73</v>
+      </c>
+      <c r="I73" t="s">
+        <v>81</v>
+      </c>
+      <c r="J73" t="s">
+        <v>82</v>
+      </c>
+      <c r="K73" t="s">
+        <v>37</v>
+      </c>
+      <c r="L73" t="s">
+        <v>38</v>
+      </c>
+      <c r="M73" t="s">
+        <v>39</v>
+      </c>
+      <c r="N73" t="s">
+        <v>40</v>
+      </c>
+      <c r="O73" t="s">
+        <v>41</v>
+      </c>
+      <c r="P73" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>43</v>
+      </c>
+      <c r="R73" t="s">
+        <v>54</v>
+      </c>
+      <c r="S73" t="s">
+        <v>45</v>
+      </c>
+      <c r="T73" t="s">
+        <v>55</v>
+      </c>
+      <c r="U73" s="1">
+        <v>9723873618.91</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74" t="s">
+        <v>73</v>
+      </c>
+      <c r="E74" t="s">
+        <v>74</v>
+      </c>
+      <c r="F74" t="s">
+        <v>75</v>
+      </c>
+      <c r="G74" t="s">
+        <v>76</v>
+      </c>
+      <c r="H74" t="s">
+        <v>73</v>
+      </c>
+      <c r="I74" t="s">
+        <v>81</v>
+      </c>
+      <c r="J74" t="s">
+        <v>82</v>
+      </c>
+      <c r="K74" t="s">
+        <v>37</v>
+      </c>
+      <c r="L74" t="s">
+        <v>38</v>
+      </c>
+      <c r="M74" t="s">
+        <v>39</v>
+      </c>
+      <c r="N74" t="s">
+        <v>40</v>
+      </c>
+      <c r="O74" t="s">
+        <v>41</v>
+      </c>
+      <c r="P74" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>43</v>
+      </c>
+      <c r="R74" t="s">
+        <v>56</v>
+      </c>
+      <c r="S74" t="s">
+        <v>45</v>
+      </c>
+      <c r="T74" t="s">
+        <v>57</v>
+      </c>
+      <c r="U74" s="1">
+        <v>12364120249.54</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>27</v>
+      </c>
+      <c r="B75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C75" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" t="s">
+        <v>73</v>
+      </c>
+      <c r="E75" t="s">
+        <v>74</v>
+      </c>
+      <c r="F75" t="s">
+        <v>75</v>
+      </c>
+      <c r="G75" t="s">
+        <v>76</v>
+      </c>
+      <c r="H75" t="s">
+        <v>73</v>
+      </c>
+      <c r="I75" t="s">
+        <v>81</v>
+      </c>
+      <c r="J75" t="s">
+        <v>82</v>
+      </c>
+      <c r="K75" t="s">
+        <v>37</v>
+      </c>
+      <c r="L75" t="s">
+        <v>38</v>
+      </c>
+      <c r="M75" t="s">
+        <v>39</v>
+      </c>
+      <c r="N75" t="s">
+        <v>40</v>
+      </c>
+      <c r="O75" t="s">
+        <v>41</v>
+      </c>
+      <c r="P75" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>43</v>
+      </c>
+      <c r="R75" t="s">
+        <v>58</v>
+      </c>
+      <c r="S75" t="s">
+        <v>45</v>
+      </c>
+      <c r="T75" t="s">
+        <v>59</v>
+      </c>
+      <c r="U75" s="1">
+        <v>11927717103.54</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>27</v>
+      </c>
+      <c r="B76" t="s">
+        <v>28</v>
+      </c>
+      <c r="C76" t="s">
+        <v>72</v>
+      </c>
+      <c r="D76" t="s">
+        <v>73</v>
+      </c>
+      <c r="E76" t="s">
+        <v>74</v>
+      </c>
+      <c r="F76" t="s">
+        <v>75</v>
+      </c>
+      <c r="G76" t="s">
+        <v>76</v>
+      </c>
+      <c r="H76" t="s">
+        <v>73</v>
+      </c>
+      <c r="I76" t="s">
+        <v>81</v>
+      </c>
+      <c r="J76" t="s">
+        <v>82</v>
+      </c>
+      <c r="K76" t="s">
+        <v>37</v>
+      </c>
+      <c r="L76" t="s">
+        <v>38</v>
+      </c>
+      <c r="M76" t="s">
+        <v>39</v>
+      </c>
+      <c r="N76" t="s">
+        <v>40</v>
+      </c>
+      <c r="O76" t="s">
+        <v>41</v>
+      </c>
+      <c r="P76" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>43</v>
+      </c>
+      <c r="R76" t="s">
+        <v>60</v>
+      </c>
+      <c r="S76" t="s">
+        <v>45</v>
+      </c>
+      <c r="T76" t="s">
+        <v>61</v>
+      </c>
+      <c r="U76" s="1">
+        <v>9808655344.2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>27</v>
+      </c>
+      <c r="B77" t="s">
+        <v>28</v>
+      </c>
+      <c r="C77" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" t="s">
+        <v>73</v>
+      </c>
+      <c r="E77" t="s">
+        <v>74</v>
+      </c>
+      <c r="F77" t="s">
+        <v>75</v>
+      </c>
+      <c r="G77" t="s">
+        <v>76</v>
+      </c>
+      <c r="H77" t="s">
+        <v>73</v>
+      </c>
+      <c r="I77" t="s">
+        <v>81</v>
+      </c>
+      <c r="J77" t="s">
+        <v>82</v>
+      </c>
+      <c r="K77" t="s">
+        <v>37</v>
+      </c>
+      <c r="L77" t="s">
+        <v>38</v>
+      </c>
+      <c r="M77" t="s">
+        <v>39</v>
+      </c>
+      <c r="N77" t="s">
+        <v>40</v>
+      </c>
+      <c r="O77" t="s">
+        <v>41</v>
+      </c>
+      <c r="P77" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>43</v>
+      </c>
+      <c r="R77" t="s">
+        <v>62</v>
+      </c>
+      <c r="S77" t="s">
+        <v>45</v>
+      </c>
+      <c r="T77" t="s">
+        <v>63</v>
+      </c>
+      <c r="U77" s="1">
+        <v>12375030809.84</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>27</v>
+      </c>
+      <c r="B78" t="s">
+        <v>28</v>
+      </c>
+      <c r="C78" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" t="s">
+        <v>73</v>
+      </c>
+      <c r="E78" t="s">
+        <v>74</v>
+      </c>
+      <c r="F78" t="s">
+        <v>75</v>
+      </c>
+      <c r="G78" t="s">
+        <v>76</v>
+      </c>
+      <c r="H78" t="s">
+        <v>73</v>
+      </c>
+      <c r="I78" t="s">
+        <v>81</v>
+      </c>
+      <c r="J78" t="s">
+        <v>82</v>
+      </c>
+      <c r="K78" t="s">
+        <v>37</v>
+      </c>
+      <c r="L78" t="s">
+        <v>38</v>
+      </c>
+      <c r="M78" t="s">
+        <v>39</v>
+      </c>
+      <c r="N78" t="s">
+        <v>40</v>
+      </c>
+      <c r="O78" t="s">
+        <v>41</v>
+      </c>
+      <c r="P78" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>43</v>
+      </c>
+      <c r="R78" t="s">
+        <v>64</v>
+      </c>
+      <c r="S78" t="s">
+        <v>45</v>
+      </c>
+      <c r="T78" t="s">
+        <v>65</v>
+      </c>
+      <c r="U78" s="1">
+        <v>12024047664.12</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>27</v>
+      </c>
+      <c r="B79" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79" t="s">
+        <v>72</v>
+      </c>
+      <c r="D79" t="s">
+        <v>73</v>
+      </c>
+      <c r="E79" t="s">
+        <v>74</v>
+      </c>
+      <c r="F79" t="s">
+        <v>75</v>
+      </c>
+      <c r="G79" t="s">
+        <v>76</v>
+      </c>
+      <c r="H79" t="s">
+        <v>73</v>
+      </c>
+      <c r="I79" t="s">
+        <v>81</v>
+      </c>
+      <c r="J79" t="s">
+        <v>82</v>
+      </c>
+      <c r="K79" t="s">
+        <v>37</v>
+      </c>
+      <c r="L79" t="s">
+        <v>38</v>
+      </c>
+      <c r="M79" t="s">
+        <v>39</v>
+      </c>
+      <c r="N79" t="s">
+        <v>40</v>
+      </c>
+      <c r="O79" t="s">
+        <v>41</v>
+      </c>
+      <c r="P79" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>43</v>
+      </c>
+      <c r="R79" t="s">
+        <v>66</v>
+      </c>
+      <c r="S79" t="s">
+        <v>45</v>
+      </c>
+      <c r="T79" t="s">
+        <v>67</v>
+      </c>
+      <c r="U79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>27</v>
+      </c>
+      <c r="B80" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" t="s">
+        <v>72</v>
+      </c>
+      <c r="D80" t="s">
+        <v>73</v>
+      </c>
+      <c r="E80" t="s">
+        <v>74</v>
+      </c>
+      <c r="F80" t="s">
+        <v>75</v>
+      </c>
+      <c r="G80" t="s">
+        <v>76</v>
+      </c>
+      <c r="H80" t="s">
+        <v>73</v>
+      </c>
+      <c r="I80" t="s">
+        <v>81</v>
+      </c>
+      <c r="J80" t="s">
+        <v>82</v>
+      </c>
+      <c r="K80" t="s">
+        <v>37</v>
+      </c>
+      <c r="L80" t="s">
+        <v>38</v>
+      </c>
+      <c r="M80" t="s">
+        <v>39</v>
+      </c>
+      <c r="N80" t="s">
+        <v>40</v>
+      </c>
+      <c r="O80" t="s">
+        <v>41</v>
+      </c>
+      <c r="P80" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>43</v>
+      </c>
+      <c r="R80" t="s">
+        <v>68</v>
+      </c>
+      <c r="S80" t="s">
+        <v>45</v>
+      </c>
+      <c r="T80" t="s">
+        <v>69</v>
+      </c>
+      <c r="U80" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>